<commit_message>
Updating my files (report)
</commit_message>
<xml_diff>
--- a/components and prices.xlsx
+++ b/components and prices.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\courses_main\1-courses\univer courses\FYP_project\0-Bills and material\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study Materials\1-Main\univer courses\12-FYP_project\0-Bills and material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD7408D-988B-4C4C-AA7B-9B4AFD7901D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354A4A20-0D73-483C-8FA5-DC500CFF3874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{17E49610-B540-4250-B9CB-8CBA1A5A2175}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="178">
   <si>
     <t>Component</t>
   </si>
@@ -571,6 +571,9 @@
   </si>
   <si>
     <t>Resettable Fuse | RXE 160  1.6A</t>
+  </si>
+  <si>
+    <t>PCB</t>
   </si>
 </sst>
 </file>
@@ -3711,8 +3714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CFF947-6E4A-4ADF-B354-FB1D3677D3C8}">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B44" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="153" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4392,9 +4395,8 @@
       <c r="I31" s="68"/>
     </row>
     <row r="32" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="22">
-        <f ca="1">A32</f>
-        <v>0</v>
+      <c r="A32" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="B32" s="16">
         <v>2</v>
@@ -5651,23 +5653,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1f1ae716-0de6-4d9c-b665-05bafdb27fd9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007CDA81A3FCDBA54387E6359357A72912" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4d721a7bd504c9ed94e8e0a518c5578f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1f1ae716-0de6-4d9c-b665-05bafdb27fd9" xmlns:ns4="b276ef11-b451-45ae-8d2e-3523693103af" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0895d8ba4e178d9327dcf2053d150154" ns3:_="" ns4:_="">
     <xsd:import namespace="1f1ae716-0de6-4d9c-b665-05bafdb27fd9"/>
@@ -5920,32 +5905,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F016DCB0-E444-427F-83E8-4069DAC707D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b276ef11-b451-45ae-8d2e-3523693103af"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1f1ae716-0de6-4d9c-b665-05bafdb27fd9"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8342DE9F-6A09-4AD9-89E8-73E3C816B80E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1f1ae716-0de6-4d9c-b665-05bafdb27fd9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7D57ED-3BF6-4A33-A077-EA0B0606C773}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5962,4 +5939,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8342DE9F-6A09-4AD9-89E8-73E3C816B80E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F016DCB0-E444-427F-83E8-4069DAC707D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b276ef11-b451-45ae-8d2e-3523693103af"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1f1ae716-0de6-4d9c-b665-05bafdb27fd9"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>